<commit_message>
Added 4 more ADCs in the family (these ones I actually have rn)
</commit_message>
<xml_diff>
--- a/Misc Stuff/Library Research/ADCs/ADS131M0X/parts.xlsx
+++ b/Misc Stuff/Library Research/ADCs/ADS131M0X/parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Misc Stuff\Library Research\ADCs\ADS131M0X\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Danakil_KiCad_DB\Misc Stuff\Library Research\ADCs\ADS131M0X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACBFEBAB-07E0-47B5-9129-8210BF0BC255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56808875-49A8-446A-8762-55F9963A355E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12740" yWindow="3550" windowWidth="13560" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>ADS131M02IPWR</t>
   </si>
@@ -106,6 +106,33 @@
   </si>
   <si>
     <t>296-ADS131M08IRSNRCT-ND</t>
+  </si>
+  <si>
+    <t>AMC131M01DFMR</t>
+  </si>
+  <si>
+    <t>AMC131M03DFMR</t>
+  </si>
+  <si>
+    <t>ADS131B02QPWRQ1</t>
+  </si>
+  <si>
+    <t>ADS131B04QPWRQ1</t>
+  </si>
+  <si>
+    <t>296-AMC131M01DFMRCT-ND</t>
+  </si>
+  <si>
+    <t>20-SOIC</t>
+  </si>
+  <si>
+    <t>296-AMC131M03DFMRCT-ND</t>
+  </si>
+  <si>
+    <t>296-ADS131B02QPWRQ1CT-ND</t>
+  </si>
+  <si>
+    <t>296-ADS131B04QPWRQ1CT-ND</t>
   </si>
 </sst>
 </file>
@@ -423,20 +450,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:D12"/>
+  <dimension ref="A3:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -450,7 +477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -464,7 +491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -478,7 +505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -492,7 +519,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -506,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -520,7 +547,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -534,7 +561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -548,7 +575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -562,7 +589,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -574,6 +601,62 @@
       </c>
       <c r="D12" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>